<commit_message>
more updates to intro
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>instruct_text</t>
   </si>
@@ -39,26 +39,7 @@
     <t>There are 8 possible jobs you could be asked to simulate.</t>
   </si>
   <si>
-    <t xml:space="preserve">In addition, your task will be to answer job-related questions.
-</t>
-  </si>
-  <si>
-    <t>There are four question per job.</t>
-  </si>
-  <si>
-    <t>You will have to try to memorize these questions and then remember your answers to the questions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You will asked about the answers to these questions at end of the experiment. </t>
-  </si>
-  <si>
-    <t>In order to help you memorize the questions, there will be a short quiz on them before the actual task begins.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In addition, before each story, there will be a reminder of what these questions are.  </t>
-  </si>
-  <si>
-    <t>Press the space bar to begin learning the jobs and the questions for each one.</t>
+    <t>These jobs are as follows:</t>
   </si>
 </sst>
 </file>
@@ -117,7 +98,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -230,13 +211,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -274,6 +292,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -301,6 +328,7 @@
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1446,7 +1474,7 @@
       <c r="G6" s="12"/>
     </row>
     <row r="7" ht="116.05" customHeight="1">
-      <c r="A7" t="s" s="10">
+      <c r="A7" t="s" s="13">
         <v>8</v>
       </c>
       <c r="B7" s="11"/>
@@ -1457,9 +1485,7 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" ht="116.05" customHeight="1">
-      <c r="A8" t="s" s="10">
-        <v>9</v>
-      </c>
+      <c r="A8" s="14"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1468,9 +1494,7 @@
       <c r="G8" s="12"/>
     </row>
     <row r="9" ht="116.05" customHeight="1">
-      <c r="A9" t="s" s="10">
-        <v>10</v>
-      </c>
+      <c r="A9" s="14"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1479,9 +1503,7 @@
       <c r="G9" s="12"/>
     </row>
     <row r="10" ht="116.05" customHeight="1">
-      <c r="A10" t="s" s="10">
-        <v>11</v>
-      </c>
+      <c r="A10" s="14"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -1490,9 +1512,7 @@
       <c r="G10" s="12"/>
     </row>
     <row r="11" ht="155.55" customHeight="1">
-      <c r="A11" t="s" s="10">
-        <v>12</v>
-      </c>
+      <c r="A11" s="14"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -1501,9 +1521,7 @@
       <c r="G11" s="12"/>
     </row>
     <row r="12" ht="155.55" customHeight="1">
-      <c r="A12" t="s" s="10">
-        <v>13</v>
-      </c>
+      <c r="A12" s="14"/>
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1512,9 +1530,7 @@
       <c r="G12" s="12"/>
     </row>
     <row r="13" ht="68.05" customHeight="1">
-      <c r="A13" t="s" s="10">
-        <v>14</v>
-      </c>
+      <c r="A13" s="15"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -1523,7 +1539,7 @@
       <c r="G13" s="12"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="13"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1532,7 +1548,7 @@
       <c r="G14" s="12"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="13"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -1541,7 +1557,7 @@
       <c r="G15" s="12"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="13"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -1550,7 +1566,7 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="13"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -1559,7 +1575,7 @@
       <c r="G17" s="12"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="13"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
@@ -1568,7 +1584,7 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="13"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="11"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -1577,7 +1593,7 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="13"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -1586,7 +1602,7 @@
       <c r="G20" s="12"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="13"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -1595,7 +1611,7 @@
       <c r="G21" s="12"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="13"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -1604,7 +1620,7 @@
       <c r="G22" s="12"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="13"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -1613,7 +1629,7 @@
       <c r="G23" s="12"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="13"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -1622,7 +1638,7 @@
       <c r="G24" s="12"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="13"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="11"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
@@ -1631,7 +1647,7 @@
       <c r="G25" s="12"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="13"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="11"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>

</xml_diff>